<commit_message>
Se tiene el filtro para temperatura, tambien ya incluí el envio de data en formato de archivo
</commit_message>
<xml_diff>
--- a/datastatic/blacklist.xlsx
+++ b/datastatic/blacklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snayd\Desktop\Dalia\gestion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snayd\Desktop\Dalia\gestion\datastatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9A5BD-F26B-4D12-9245-F3B2534C0FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA80F82-D908-4ECD-9642-133F1CEBC8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID_UNICO</t>
   </si>
   <si>
     <t>LI01649</t>
+  </si>
+  <si>
+    <t>LI00353</t>
   </si>
 </sst>
 </file>
@@ -348,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -369,6 +372,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>